<commit_message>
Some new files in marketing folder
</commit_message>
<xml_diff>
--- a/Google/sales/pixel.xlsx
+++ b/Google/sales/pixel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hitesh Somani\Documents\hobby_projects\nlp_document_finder\nlp_document_finder\Google\sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E04B14E-698D-40FE-8C2C-CCBCAE65413C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AC4911-53E7-46B4-9036-EFE482E0E3EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{2198444F-CEFF-4941-A69D-0ED224E784D6}"/>
   </bookViews>
@@ -30,6 +30,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>This is demo file</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,7 +392,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>